<commit_message>
Updated OOH Stamping with Tag invoices
</commit_message>
<xml_diff>
--- a/Broadcast S9/Brodcast Email to S9 Dispatcher/Data/Config.xlsx
+++ b/Broadcast S9/Brodcast Email to S9 Dispatcher/Data/Config.xlsx
@@ -3880,10 +3880,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045A9A53AB2AD7C409EFC96CC55961B83" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1cca1f8f06752839a5d2a2aaf5a51db7">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="649a79cd-06e4-47a3-aac9-21cb806f3675" xmlns:ns3="7f25b792-b2ba-4b5c-8669-b39a27555406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c3ef14356e556b93afe382ac3fbbcf07" ns2:_="" ns3:_="">
-    <xsd:import namespace="649a79cd-06e4-47a3-aac9-21cb806f3675"/>
-    <xsd:import namespace="7f25b792-b2ba-4b5c-8669-b39a27555406"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D123EB44872014A9CBA28754C030F45" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b63aef4ab9a0554846bbd80426a442de">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b" xmlns:ns3="d1eda545-557d-4822-aebd-96c436cdfdd2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="025929af57d157df69a05cd96369afaf" ns2:_="" ns3:_="">
+    <xsd:import namespace="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b"/>
+    <xsd:import namespace="d1eda545-557d-4822-aebd-96c436cdfdd2"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -3892,12 +3892,17 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:Pic" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
@@ -3907,7 +3912,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="649a79cd-06e4-47a3-aac9-21cb806f3675" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -3920,7 +3925,17 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -3932,17 +3947,41 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Pic" ma:index="19" nillable="true" ma:displayName="Pic" ma:format="Image" ma:internalName="Pic">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="cb8c6112-a551-416c-b446-07c3fc3d0d42" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="cb8c6112-a551-416c-b446-07c3fc3d0d42" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -3950,10 +3989,10 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7f25b792-b2ba-4b5c-8669-b39a27555406" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d1eda545-557d-4822-aebd-96c436cdfdd2" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -3972,14 +4011,14 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="18" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{2e954b58-32a8-4cab-baf9-92d5046718f0}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7f25b792-b2ba-4b5c-8669-b39a27555406">
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{818068d8-5dd5-4fbd-ae53-d04ba5fbca96}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d1eda545-557d-4822-aebd-96c436cdfdd2">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -4102,22 +4141,26 @@
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <TaxCatchAll xmlns="7f25b792-b2ba-4b5c-8669-b39a27555406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="649a79cd-06e4-47a3-aac9-21cb806f3675">
+    <Pic xmlns="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Pic>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a0a8f4a1-fec1-45cc-8c4b-70028d19f88b">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d1eda545-557d-4822-aebd-96c436cdfdd2" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F834B39-6DE6-4A6E-9C53-C70A2967A4A9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4643092-2DE2-41C3-918A-C541CECFF7C4}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C537615-50A5-4863-ACE8-96935C0575CA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD4827B2-4DFA-4236-93AA-25AB43FCF814}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36041115-E152-4F59-BAB4-B288BFA746B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD3CEC8C-C918-4012-8E8E-C6805867A8D8}"/>
 </file>
</xml_diff>

<commit_message>
Updated OOH S9 code to Prod DB
</commit_message>
<xml_diff>
--- a/Broadcast S9/Brodcast Email to S9 Dispatcher/Data/Config.xlsx
+++ b/Broadcast S9/Brodcast Email to S9 Dispatcher/Data/Config.xlsx
@@ -4154,13 +4154,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4643092-2DE2-41C3-918A-C541CECFF7C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{602A1A6E-5085-4B27-A9FE-F82F2B7B35AB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD4827B2-4DFA-4236-93AA-25AB43FCF814}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5698786C-97C3-4969-A57B-0968CEA042B4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD3CEC8C-C918-4012-8E8E-C6805867A8D8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A7FE59C-04DB-4976-99C7-D934ED5B5B4D}"/>
 </file>
</xml_diff>

<commit_message>
Added Updated codes for all S9 process
</commit_message>
<xml_diff>
--- a/Broadcast S9/Brodcast Email to S9 Dispatcher/Data/Config.xlsx
+++ b/Broadcast S9/Brodcast Email to S9 Dispatcher/Data/Config.xlsx
@@ -4154,13 +4154,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{602A1A6E-5085-4B27-A9FE-F82F2B7B35AB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E783FBC-F4AA-42B8-B066-9B96FC100506}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5698786C-97C3-4969-A57B-0968CEA042B4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C1392A9-FE87-4324-B7D8-9356AC07543C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A7FE59C-04DB-4976-99C7-D934ED5B5B4D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0BB41A9-2896-42F6-9A71-5FE579048F5E}"/>
 </file>
</xml_diff>